<commit_message>
include errors for incorrect data entry
</commit_message>
<xml_diff>
--- a/data/transformed_data.xlsx
+++ b/data/transformed_data.xlsx
@@ -515,7 +515,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F2" t="n">
         <v>42</v>
@@ -527,13 +527,13 @@
         <v>50</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.9770609318996425</v>
+        <v>-1.492114695340502</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.1757966344432509</v>
+        <v>-0.5420694593626935</v>
       </c>
       <c r="K2" t="n">
-        <v>0.6447697250981795</v>
+        <v>0.2988218493395215</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
@@ -644,7 +644,7 @@
         <v>5776</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
         <v>12</v>
@@ -659,13 +659,13 @@
         <v>60</v>
       </c>
       <c r="I5" t="n">
-        <v>2.891039426523297</v>
+        <v>2.908960573476702</v>
       </c>
       <c r="J5" t="n">
-        <v>-3.759040458288578</v>
+        <v>-3.248120300751879</v>
       </c>
       <c r="K5" t="n">
-        <v>1.493038200642628</v>
+        <v>2.272045697965013</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
@@ -688,7 +688,7 @@
         <v>2500</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
         <v>15</v>
@@ -703,13 +703,13 @@
         <v>60</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9559139784946242</v>
+        <v>0.9738351254480289</v>
       </c>
       <c r="J6" t="n">
-        <v>-2.663802363050485</v>
+        <v>-2.152882205513786</v>
       </c>
       <c r="K6" t="n">
-        <v>1.351303106033559</v>
+        <v>2.130310603355944</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
adjusted output data after rerunning script
</commit_message>
<xml_diff>
--- a/data/transformed_data.xlsx
+++ b/data/transformed_data.xlsx
@@ -533,7 +533,7 @@
         <v>-0.1757966344432509</v>
       </c>
       <c r="K2" t="n">
-        <v>0.6447697250981795</v>
+        <v>-0.9132452695465898</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
@@ -577,7 +577,7 @@
         <v>-3.232008592910849</v>
       </c>
       <c r="K3" t="n">
-        <v>-2.078900392716887</v>
+        <v>-5.194930382006427</v>
       </c>
       <c r="L3" t="n">
         <v>1</v>
@@ -621,7 +621,7 @@
         <v>1.135338345864661</v>
       </c>
       <c r="K4" t="n">
-        <v>2.546590503391646</v>
+        <v>-0.5694394858978932</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
@@ -665,7 +665,7 @@
         <v>-3.759040458288578</v>
       </c>
       <c r="K5" t="n">
-        <v>1.493038200642628</v>
+        <v>-0.0649767940021416</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
@@ -709,7 +709,7 @@
         <v>-2.663802363050485</v>
       </c>
       <c r="K6" t="n">
-        <v>1.351303106033559</v>
+        <v>-0.2067118886112105</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>

</xml_diff>